<commit_message>
function well still miss jira linked function
</commit_message>
<xml_diff>
--- a/Test_Jira/jira_input_v2.1.0.xlsx
+++ b/Test_Jira/jira_input_v2.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtcelec2\Desktop\kaiheng\JIRA_Auto\Test_Jira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875543BF-CB29-401F-A6B3-C01F1CFA5B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA5524E-8C3E-414B-A253-1060397F53C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16284" yWindow="-2724" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>DeviceID</t>
   </si>
@@ -52,21 +52,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Marja Blasé</t>
-  </si>
-  <si>
-    <t>Yan Chen</t>
-  </si>
-  <si>
-    <t>Fabio De Leo</t>
-  </si>
-  <si>
-    <t>Lyuba Goundareva</t>
-  </si>
-  <si>
-    <t>Melissa Cuthill</t>
-  </si>
-  <si>
     <t>Hi, note 1</t>
   </si>
   <si>
@@ -91,35 +76,23 @@
     <t>Hi, note 8</t>
   </si>
   <si>
-    <t>01/07/2021</t>
-  </si>
-  <si>
-    <t>01/30/2021</t>
-  </si>
-  <si>
-    <t>01/17/2022</t>
-  </si>
-  <si>
-    <t>03/17/2021</t>
-  </si>
-  <si>
-    <t>04/07/2021</t>
-  </si>
-  <si>
-    <t>01/14/2021</t>
-  </si>
-  <si>
-    <t>02/21/2021</t>
-  </si>
-  <si>
-    <t>11/22/2021</t>
+    <t>button@uvic.ca</t>
+  </si>
+  <si>
+    <t>aalbu@uvic.ca</t>
+  </si>
+  <si>
+    <t>nbailly@uvic.ca</t>
+  </si>
+  <si>
+    <t>mtcelec2@uvic.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -162,6 +135,12 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -242,10 +221,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,24 +259,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,8 +511,8 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -530,7 +526,7 @@
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,14 +562,14 @@
       <c r="A2" s="6">
         <v>31379</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="23">
+        <v>44203</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>15</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
@@ -585,14 +581,14 @@
       <c r="A3" s="11">
         <v>22773</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>24</v>
+      <c r="B3" s="23">
+        <v>44226</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
@@ -604,14 +600,14 @@
       <c r="A4" s="12">
         <v>30799</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>17</v>
+      <c r="B4" s="23">
+        <v>44522</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
@@ -623,14 +619,14 @@
       <c r="A5" s="7">
         <v>10604</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>18</v>
+      <c r="B5" s="23">
+        <v>44510</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -642,14 +638,14 @@
       <c r="A6" s="13">
         <v>23039</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="23">
+        <v>44440</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>19</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
@@ -661,14 +657,14 @@
       <c r="A7" s="12">
         <v>9</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="B7" s="23">
+        <v>44429</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
@@ -680,14 +676,14 @@
       <c r="A8" s="6">
         <v>40</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="17" t="s">
+      <c r="B8" s="23">
+        <v>44285</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>21</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
@@ -699,14 +695,14 @@
       <c r="A9" s="6">
         <v>10</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>22</v>
+      <c r="B9" s="23">
+        <v>44309</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
@@ -715,21 +711,21 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -741,7 +737,17 @@
     <mergeCell ref="A10:F10"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1EB28250-41CA-4B5B-B3C9-550174551E87}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{ABAD4DC6-5AF2-42CE-96E4-523E3EE00CDC}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{9661DEBF-4E0A-4DF7-93DE-51AD8EAB5DF9}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{11DA456E-875A-41B8-B6D4-A24856FC75B3}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{D2D458B6-7712-470F-9FF3-0741135D00BA}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{8849A7E7-5DDF-49E2-BF14-FCFD458C8E14}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{C5E110C9-6A35-44FC-9490-AA85A6F2C4C0}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{DCBC4DDF-390C-482D-80B4-F5D340C2891F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
version 2.0.4 push to save before adding GUI
</commit_message>
<xml_diff>
--- a/Test_Jira/jira_input_v2.1.0.xlsx
+++ b/Test_Jira/jira_input_v2.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtcelec2\Desktop\kaiheng\JIRA_Auto\Test_Jira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA5524E-8C3E-414B-A253-1060397F53C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFB64E7-9C02-434A-ADCD-34F62532B39F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16284" yWindow="-2724" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>DeviceID</t>
   </si>
@@ -52,15 +52,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Hi, note 1</t>
-  </si>
-  <si>
-    <t>Hi, note 2</t>
-  </si>
-  <si>
-    <t>Hi, note 3</t>
-  </si>
-  <si>
     <t>Hi, note 4</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
     <t>Hi, note 7</t>
   </si>
   <si>
-    <t>Hi, note 8</t>
-  </si>
-  <si>
     <t>button@uvic.ca</t>
   </si>
   <si>
@@ -86,6 +74,30 @@
   </si>
   <si>
     <t>mtcelec2@uvic.ca</t>
+  </si>
+  <si>
+    <t>EN-54135</t>
+  </si>
+  <si>
+    <t>EN-54134</t>
+  </si>
+  <si>
+    <t>EN-54131</t>
+  </si>
+  <si>
+    <t>EN-54121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi, I know this is hard </t>
+  </si>
+  <si>
+    <t>Hi, OK, we should work on the EN-54134</t>
+  </si>
+  <si>
+    <t>Hi, COOPPPPPPP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi, Customers are required to wear a face covering in all of our stores. </t>
   </si>
 </sst>
 </file>
@@ -511,15 +523,16 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.42578125" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="26.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="101.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="44.28515625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
@@ -566,12 +579,14 @@
         <v>44203</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -585,12 +600,14 @@
         <v>44226</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="9"/>
@@ -604,10 +621,10 @@
         <v>44522</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
@@ -623,10 +640,10 @@
         <v>44510</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
@@ -642,10 +659,10 @@
         <v>44440</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
@@ -661,12 +678,14 @@
         <v>44429</v>
       </c>
       <c r="C7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
@@ -680,12 +699,14 @@
         <v>44285</v>
       </c>
       <c r="C8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
@@ -699,10 +720,10 @@
         <v>44309</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>

</xml_diff>